<commit_message>
Ajustes dashboard y plan de trabajo
</commit_message>
<xml_diff>
--- a/public/importacion/Plantilla Empleados.xlsx
+++ b/public/importacion/Plantilla Empleados.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="109">
   <si>
     <t>TipoIdentificacion_idTipoIdentificacion</t>
   </si>
@@ -959,10 +959,10 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1482,75 +1482,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.140625" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" customWidth="1"/>
-    <col min="25" max="25" width="16.7109375" customWidth="1"/>
-    <col min="26" max="26" width="17.85546875" customWidth="1"/>
-    <col min="27" max="27" width="34.85546875" customWidth="1"/>
-    <col min="28" max="28" width="29.28515625" customWidth="1"/>
-    <col min="29" max="29" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.125" customWidth="1"/>
+    <col min="24" max="24" width="15.75" customWidth="1"/>
+    <col min="25" max="25" width="16.75" customWidth="1"/>
+    <col min="26" max="26" width="17.875" customWidth="1"/>
+    <col min="27" max="27" width="34.875" customWidth="1"/>
+    <col min="28" max="28" width="29.25" customWidth="1"/>
+    <col min="29" max="29" width="29.125" customWidth="1"/>
     <col min="32" max="32" width="25" customWidth="1"/>
-    <col min="34" max="34" width="18.85546875" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" customWidth="1"/>
-    <col min="36" max="36" width="28.7109375" customWidth="1"/>
-    <col min="37" max="37" width="24.85546875" customWidth="1"/>
-    <col min="38" max="38" width="22.7109375" customWidth="1"/>
-    <col min="39" max="39" width="31.42578125" customWidth="1"/>
-    <col min="40" max="40" width="24.42578125" customWidth="1"/>
+    <col min="34" max="34" width="18.875" customWidth="1"/>
+    <col min="35" max="35" width="21.875" customWidth="1"/>
+    <col min="36" max="36" width="28.75" customWidth="1"/>
+    <col min="37" max="37" width="24.875" customWidth="1"/>
+    <col min="38" max="38" width="22.75" customWidth="1"/>
+    <col min="39" max="39" width="31.375" customWidth="1"/>
+    <col min="40" max="40" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1667,7 +1667,7 @@
       <c r="AL3" t="s">
         <v>64</v>
       </c>
-      <c r="AM3" s="10" t="s">
+      <c r="AM3" s="9" t="s">
         <v>65</v>
       </c>
       <c r="AN3" t="s">
@@ -1816,7 +1816,9 @@
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
+      <c r="AL5" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="AM5" s="3"/>
       <c r="AN5" s="3"/>
     </row>
@@ -1893,13 +1895,19 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1909,22 +1917,22 @@
       <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1935,22 +1943,22 @@
       <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1961,59 +1969,60 @@
       <c r="B3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios generales y plan trabajo formulario
</commit_message>
<xml_diff>
--- a/public/importacion/Plantilla Empleados.xlsx
+++ b/public/importacion/Plantilla Empleados.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="130">
   <si>
     <t>TipoIdentificacion_idTipoIdentificacion</t>
   </si>
@@ -408,6 +408,69 @@
   </si>
   <si>
     <t>Resp. Logica</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Camila</t>
+  </si>
+  <si>
+    <t>Baba</t>
+  </si>
+  <si>
+    <t>Pum</t>
+  </si>
+  <si>
+    <t>asdfg</t>
+  </si>
+  <si>
+    <t>*01*</t>
+  </si>
+  <si>
+    <t>Calle</t>
+  </si>
+  <si>
+    <t>05001</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>3456</t>
+  </si>
+  <si>
+    <t>435</t>
+  </si>
+  <si>
+    <t>saa</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Jugar</t>
+  </si>
+  <si>
+    <t>111111111</t>
   </si>
 </sst>
 </file>
@@ -949,7 +1012,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -963,6 +1026,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1483,7 +1547,7 @@
   <dimension ref="A1:AN5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,28 +1861,120 @@
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="1">
+        <v>42699</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J5" s="2"/>
-      <c r="M5" s="4"/>
-      <c r="S5" s="1"/>
-      <c r="W5" s="1"/>
+      <c r="K5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="1">
+        <v>34919</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="W5" s="1">
+        <v>42370</v>
+      </c>
       <c r="X5" s="1"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
+      <c r="Y5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
+      <c r="AN5" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
@@ -1833,7 +1989,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$B$2:$B$3</xm:f>

</xml_diff>

<commit_message>
Resultado de examen medico y plantilla tercero
</commit_message>
<xml_diff>
--- a/public/importacion/Plantilla Empleados.xlsx
+++ b/public/importacion/Plantilla Empleados.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
   <si>
     <t>TipoIdentificacion_idTipoIdentificacion</t>
   </si>
@@ -408,69 +408,6 @@
   </si>
   <si>
     <t>Resp. Logica</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>Camila</t>
-  </si>
-  <si>
-    <t>Baba</t>
-  </si>
-  <si>
-    <t>Pum</t>
-  </si>
-  <si>
-    <t>asdfg</t>
-  </si>
-  <si>
-    <t>*01*</t>
-  </si>
-  <si>
-    <t>Calle</t>
-  </si>
-  <si>
-    <t>05001</t>
-  </si>
-  <si>
-    <t>345</t>
-  </si>
-  <si>
-    <t>456</t>
-  </si>
-  <si>
-    <t>3456</t>
-  </si>
-  <si>
-    <t>435</t>
-  </si>
-  <si>
-    <t>saa</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Jugar</t>
-  </si>
-  <si>
-    <t>111111111</t>
   </si>
 </sst>
 </file>
@@ -1023,10 +960,10 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1547,7 +1484,7 @@
   <dimension ref="A1:AN5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,30 +1528,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1861,120 +1798,29 @@
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" s="1">
-        <v>42699</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S5" s="1">
-        <v>34919</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="W5" s="1">
-        <v>42370</v>
-      </c>
+      <c r="M5" s="4"/>
+      <c r="S5" s="1"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC5" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE5" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG5" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI5" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ5" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AL5" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
       <c r="AM5" s="3"/>
-      <c r="AN5" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="AN5" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
@@ -1989,7 +1835,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$B$2:$B$3</xm:f>

</xml_diff>

<commit_message>
mejoras plan trabajo y excel terceros
</commit_message>
<xml_diff>
--- a/public/importacion/Plantilla Empleados.xlsx
+++ b/public/importacion/Plantilla Empleados.xlsx
@@ -20,7 +20,7 @@
     <author>Andres Sierra</author>
   </authors>
   <commentList>
-    <comment ref="Y3" authorId="0">
+    <comment ref="Y9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF3" authorId="0">
+    <comment ref="AF9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="114">
   <si>
     <t>TipoIdentificacion_idTipoIdentificacion</t>
   </si>
@@ -113,9 +113,6 @@
     <t>imagenTercero</t>
   </si>
   <si>
-    <t>tipoTercero</t>
-  </si>
-  <si>
     <t>direccionTercero</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Foto</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
     <t>Dirección</t>
   </si>
   <si>
@@ -408,6 +402,27 @@
   </si>
   <si>
     <t>Resp. Logica</t>
+  </si>
+  <si>
+    <t>Convenciones de Títulos</t>
+  </si>
+  <si>
+    <t>Código correspondiente con maestro del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dato Obligatorio </t>
+  </si>
+  <si>
+    <t>Lista de Selección</t>
+  </si>
+  <si>
+    <t>Valor Opcional</t>
+  </si>
+  <si>
+    <t>Centro de Costos</t>
+  </si>
+  <si>
+    <t>CentroCosto_idCentroCosto</t>
   </si>
 </sst>
 </file>
@@ -417,7 +432,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,13 +569,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -586,6 +594,51 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -774,7 +827,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -904,6 +957,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -949,7 +1039,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -957,11 +1047,37 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1009,10 +1125,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="39">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1141,20 +1254,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A3:AN5" totalsRowShown="0">
-  <autoFilter ref="A3:AN5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A9:AN11" totalsRowShown="0">
+  <autoFilter ref="A9:AN11"/>
   <tableColumns count="40">
-    <tableColumn id="2" name="Tipo Identificacion" dataDxfId="39"/>
-    <tableColumn id="3" name="Documento No." dataDxfId="38"/>
-    <tableColumn id="4" name="Primer Nombre" dataDxfId="37"/>
-    <tableColumn id="5" name="Segundo Nombre" dataDxfId="36"/>
-    <tableColumn id="6" name="Primer Apellido" dataDxfId="35"/>
-    <tableColumn id="7" name="Segundo Apellido" dataDxfId="34"/>
-    <tableColumn id="8" name="Nombre Completo " dataDxfId="33"/>
-    <tableColumn id="9" name="Fecha de Creación" dataDxfId="32"/>
-    <tableColumn id="10" name="Estado" dataDxfId="31"/>
-    <tableColumn id="11" name="Foto" dataDxfId="30"/>
-    <tableColumn id="12" name="Tipo" dataDxfId="29"/>
+    <tableColumn id="2" name="Tipo Identificacion" dataDxfId="38"/>
+    <tableColumn id="3" name="Documento No." dataDxfId="37"/>
+    <tableColumn id="4" name="Primer Nombre" dataDxfId="36"/>
+    <tableColumn id="5" name="Segundo Nombre" dataDxfId="35"/>
+    <tableColumn id="6" name="Primer Apellido" dataDxfId="34"/>
+    <tableColumn id="7" name="Segundo Apellido" dataDxfId="33"/>
+    <tableColumn id="8" name="Nombre Completo " dataDxfId="32"/>
+    <tableColumn id="9" name="Fecha de Creación" dataDxfId="31"/>
+    <tableColumn id="10" name="Estado" dataDxfId="30"/>
+    <tableColumn id="11" name="Foto" dataDxfId="29"/>
     <tableColumn id="13" name="Dirección" dataDxfId="28"/>
     <tableColumn id="14" name="Ciudad" dataDxfId="27"/>
     <tableColumn id="15" name="Teléfono" dataDxfId="26"/>
@@ -1166,6 +1278,7 @@
     <tableColumn id="21" name="Correo Electrónico" dataDxfId="20"/>
     <tableColumn id="22" name="Página Web" dataDxfId="19"/>
     <tableColumn id="23" name="Cargo" dataDxfId="18"/>
+    <tableColumn id="12" name="Centro de Costos"/>
     <tableColumn id="1" name="Fecha Ingreso" dataDxfId="17"/>
     <tableColumn id="24" name="Fecha Retiro" dataDxfId="16"/>
     <tableColumn id="25" name="Tipo Contrato" dataDxfId="15"/>
@@ -1185,7 +1298,7 @@
     <tableColumn id="39" name="Frecuencia" dataDxfId="1"/>
     <tableColumn id="40" name="Consume Cigarrillo" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
       <x14:table altText="Datos del Tercero" altTextSummary="Permite ingresar la información de terceros de tipo proveedor para cargar el sistema de información SISOFT"/>
@@ -1481,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN5"/>
+  <dimension ref="A1:AN11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,17 +1612,17 @@
     <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21" style="3" customWidth="1"/>
     <col min="23" max="23" width="17.140625" customWidth="1"/>
     <col min="24" max="24" width="15.7109375" customWidth="1"/>
     <col min="25" max="25" width="16.7109375" customWidth="1"/>
@@ -1517,6 +1630,7 @@
     <col min="27" max="27" width="34.85546875" customWidth="1"/>
     <col min="28" max="28" width="29.28515625" customWidth="1"/>
     <col min="29" max="29" width="29.140625" customWidth="1"/>
+    <col min="30" max="30" width="13.85546875" customWidth="1"/>
     <col min="32" max="32" width="25" customWidth="1"/>
     <col min="34" max="34" width="18.85546875" customWidth="1"/>
     <col min="35" max="35" width="21.85546875" customWidth="1"/>
@@ -1528,304 +1642,345 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
+      <c r="A1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="9"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>66</v>
-      </c>
+      <c r="A3" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
     </row>
-    <row r="4" spans="1:40" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>84</v>
-      </c>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="M5" s="4"/>
-      <c r="S5" s="1"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
+      <c r="A5" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="W9" t="s">
+        <v>47</v>
+      </c>
+      <c r="X9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN9" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN10" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="L11" s="4"/>
+      <c r="R11" s="1"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:V1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -1840,49 +1995,49 @@
           <x14:formula1>
             <xm:f>listas!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>R5</xm:sqref>
+          <xm:sqref>Q11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I5</xm:sqref>
+          <xm:sqref>I11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Y5</xm:sqref>
+          <xm:sqref>Y11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>AD5</xm:sqref>
+          <xm:sqref>AD11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AF5</xm:sqref>
+          <xm:sqref>AF11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AH5</xm:sqref>
+          <xm:sqref>AH11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AI5</xm:sqref>
+          <xm:sqref>AI11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>AK5:AL5 AN5</xm:sqref>
+          <xm:sqref>AK11:AL11 AN11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1895,124 +2050,125 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>